<commit_message>
PCB and font updates
</commit_message>
<xml_diff>
--- a/mini_rev0/aqplus_mini_rev0_BOM.xlsx
+++ b/mini_rev0/aqplus_mini_rev0_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sph\Box\Retro\Aquarius\AquariusPlus\aquarius-plus\System\pcb\mini_rev0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36E86B4-E09D-49CC-BA78-BEAA15DD3E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4D6018-D8E7-4707-B9A0-445CF2354096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7095" yWindow="2700" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -378,9 +378,6 @@
     <t>C443416</t>
   </si>
   <si>
-    <t>C5116481</t>
-  </si>
-  <si>
     <t>C693842</t>
   </si>
   <si>
@@ -411,24 +408,15 @@
     <t>C138387</t>
   </si>
   <si>
-    <t>PJ-320B-SMT</t>
-  </si>
-  <si>
     <t>C2913203</t>
   </si>
   <si>
-    <t>C2939180</t>
-  </si>
-  <si>
     <t>Pin Headers 1x2</t>
   </si>
   <si>
     <t>JP1,JP2,JP3</t>
   </si>
   <si>
-    <t>Audio Jacks</t>
-  </si>
-  <si>
     <t>J3</t>
   </si>
   <si>
@@ -445,6 +433,18 @@
   </si>
   <si>
     <t>U1</t>
+  </si>
+  <si>
+    <t>C2905434</t>
+  </si>
+  <si>
+    <t>PJ-3200</t>
+  </si>
+  <si>
+    <t>C2689690</t>
+  </si>
+  <si>
+    <t>Audio Jack</t>
   </si>
 </sst>
 </file>
@@ -908,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -961,7 +961,7 @@
         <v>69</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3" s="6"/>
     </row>
@@ -991,7 +991,7 @@
         <v>73</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E5" s="6"/>
     </row>
@@ -1000,7 +1000,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>81</v>
@@ -1073,7 +1073,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>81</v>
@@ -1101,7 +1101,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>66</v>
@@ -1121,7 +1121,7 @@
         <v>66</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15">
@@ -1213,7 +1213,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>66</v>
@@ -1233,7 +1233,7 @@
         <v>72</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15">
@@ -1275,7 +1275,7 @@
         <v>75</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="28.5">
@@ -1303,21 +1303,21 @@
         <v>80</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15">
       <c r="A28" s="8" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="28.5">
@@ -1331,7 +1331,7 @@
         <v>76</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15">
@@ -1345,7 +1345,7 @@
         <v>68</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15">
@@ -1378,16 +1378,16 @@
     </row>
     <row r="33" spans="1:4" ht="15">
       <c r="A33" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>83</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15">
@@ -1401,7 +1401,7 @@
         <v>27</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15">
@@ -1409,13 +1409,13 @@
         <v>28</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15">
@@ -1429,7 +1429,7 @@
         <v>67</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>